<commit_message>
add image field and foreign name to books' tables
</commit_message>
<xml_diff>
--- a/DOC/API.xlsx
+++ b/DOC/API.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\QUT\Semester3\IFN711\API\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5E9036F-0EB5-4A4D-B151-47DF2E32E4EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCF9D7D0-C46C-4AB6-BB0E-B0A4BB9C6A21}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="49">
   <si>
     <t>/api/user</t>
   </si>
@@ -44,28 +45,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>username password</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>/api/user/insertUser</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">    const username = userData.username
-    const role = userData.role
-    const rolename = userData.rolename
-    const nickname = userData.nickname
-    let password = (userData.password)
-    password = genPassword(password)
-    const address = (userData.address)
-    const email = (userData.email)
-    const phone = (userData.phone)
-    const firstname = (userData.firstname)
-    const lastname = (userData.lastname)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>API</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -78,27 +61,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">    const username = (userData.username)
-    const nickname = (userData.nickname)
-    const password = (userData.password)
-    const address = (userData.address)
-    const email = (userData.email)
-    const phone = (userData.phone)
-    const firstname = (userData.firstname)
-    const lastname = (userData.lastname)
-    const experience = (userData.experience)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>/api/user/updateExp</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">    const username = (userData.username) 
-    const experience = (userData.experience)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>/api/origin/list</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -107,10 +73,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>name, author, publisher, category, trans_num</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>/api/origin/download</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -123,14 +85,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">    const id = (bookData.id)
-    const trans_num = (bookData.trans_num)
-    const download_loc = (bookData.download_loc)
-    const status = (bookData.status)
-    const status_info = (bookData.status_info)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>/api/origin/del</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -139,10 +93,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>original_id, language, translator_id, translation_reviewer_id, cultrue_reviewer_id, status</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>/api/trans/download</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -151,31 +101,157 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>/api/trans/update</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/api/trans/del</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> username 
+ nickname 
+ password 
+ address 
+ email 
+ phone 
+ firstname 
+ lastname 
+ experience </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> username  
+ experience </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> id 
+ trans_num 
+ download_loc 
+ status 
+ status_info </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  id 
+  download_loc 
+  status 
+  status_info 
+  startdate 
+  enddate 
+  translation_reviewer_id 
+  cultrue_reviewer_id 
+  copy_reviewer_id 
+  admin_id </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> username
+ role
+ rolename
+ nickname 
+ password
+ address 
+ email 
+ phone 
+ firstname 
+ lastname </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> username 
+ password</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>name
+author
+publisher
+category
+trans_num
+status</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>original_id
+language
+ translator_id
+ translation_reviewer_id
+ cultrue_reviewer_id
+ status</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>translator_id
-    const original_id = escape(bookData.original_id)
-    const language = escape(bookData.language)
-    const startdate = escape(bookData.startdate)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/api/trans/update</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">    const id = (bookData.id)
-    const download_loc = (bookData.download_loc)
-    const status = (bookData.status)
-    const status_info = (bookData.status_info)
-    const startdate = (bookData.startdate)
-    const enddate = (bookData.enddate)
-    const translation_reviewer_id = (bookData.translation_reviewer_id)
-    const cultrue_reviewer_id = (bookData.cultrue_reviewer_id)
-    const copy_reviewer_id = (bookData.copy_reviewer_id)
-    const admin_id = (bookData.admin_id)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/api/trans/del</t>
+  original_id 
+  language
+  startdate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>users</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>role</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>rolename</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>translator</t>
+  </si>
+  <si>
+    <t>translation reivewer</t>
+  </si>
+  <si>
+    <t>culture reviewer</t>
+  </si>
+  <si>
+    <t>copy reviewer</t>
+  </si>
+  <si>
+    <t>original_books</t>
+  </si>
+  <si>
+    <t>status</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>status_info</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>locked</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>normal</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>translated_books</t>
+  </si>
+  <si>
+    <t>published</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>being translated</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>being translation viewed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>being culture reviewed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>being copy reviewed</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -230,7 +306,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -238,6 +314,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -521,8 +603,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -535,54 +617,54 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="138" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="151.80000000000001" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>6</v>
-      </c>
       <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="124.2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
@@ -649,37 +731,37 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" ht="82.8" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>16</v>
+        <v>11</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="69" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="69" x14ac:dyDescent="0.25">
@@ -690,18 +772,18 @@
         <v>4</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
@@ -752,59 +834,59 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" ht="82.8" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C27" s="2" t="s">
-        <v>23</v>
+      <c r="C27" s="3" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="138" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
@@ -900,4 +982,159 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D394C38-F921-48A4-941A-34759F663F0D}">
+  <dimension ref="A1:K6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="14" customWidth="1"/>
+    <col min="3" max="3" width="22.88671875" customWidth="1"/>
+    <col min="5" max="5" width="17.109375" customWidth="1"/>
+    <col min="7" max="7" width="17.6640625" customWidth="1"/>
+    <col min="9" max="9" width="17.21875" customWidth="1"/>
+    <col min="11" max="11" width="22" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="J1" t="s">
+        <v>39</v>
+      </c>
+      <c r="K1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="5"/>
+      <c r="B2" s="4">
+        <v>0</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="5"/>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2" t="s">
+        <v>42</v>
+      </c>
+      <c r="I2" s="5"/>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="5"/>
+      <c r="B3" s="4">
+        <v>1</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" s="5"/>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
+        <v>41</v>
+      </c>
+      <c r="I3" s="5"/>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="41.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5"/>
+      <c r="B4" s="4">
+        <v>2</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4">
+        <v>2</v>
+      </c>
+      <c r="K4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5"/>
+      <c r="B5" s="4">
+        <v>3</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5">
+        <v>3</v>
+      </c>
+      <c r="K5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5"/>
+      <c r="B6" s="4">
+        <v>4</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6">
+        <v>4</v>
+      </c>
+      <c r="K6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:A6"/>
+    <mergeCell ref="E1:E6"/>
+    <mergeCell ref="I1:I6"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
remove loginCheck and fix bugs in add routes
</commit_message>
<xml_diff>
--- a/DOC/API.xlsx
+++ b/DOC/API.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\QUT\Semester3\IFN711\API\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Develop\nodejs\node_global\IFN711 Team72\DOC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCF9D7D0-C46C-4AB6-BB0E-B0A4BB9C6A21}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1864A82B-3738-4E5B-B4D3-976C69090293}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,16 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="49">
-  <si>
-    <t>/api/user</t>
-  </si>
-  <si>
-    <t>/api/origin</t>
-  </si>
-  <si>
-    <t>/api/trans</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="48">
   <si>
     <t>/api/user/login</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -252,6 +243,20 @@
   </si>
   <si>
     <t>being copy reviewed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/api/origin/add</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> name
+ publisher
+ author
+ category 
+ language
+ download_loc
+ publish_time</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -601,10 +606,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C42"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -617,365 +622,201 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="138" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="124.2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="82.8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>4</v>
+        <v>8</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="69" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="96.6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>4</v>
+        <v>1</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>4</v>
+        <v>1</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+    </row>
+    <row r="13" spans="1:3" ht="82.8" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="82.8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="138" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="69" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="69" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>23</v>
-      </c>
+    </row>
+    <row r="18" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
     </row>
     <row r="19" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>13</v>
-      </c>
+      <c r="A19" s="1"/>
     </row>
     <row r="20" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>4</v>
-      </c>
+      <c r="A20" s="1"/>
     </row>
     <row r="21" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>4</v>
-      </c>
+      <c r="A21" s="1"/>
     </row>
     <row r="22" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>4</v>
-      </c>
+      <c r="A22" s="1"/>
     </row>
     <row r="23" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>4</v>
-      </c>
+      <c r="A23" s="1"/>
     </row>
     <row r="24" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>4</v>
-      </c>
+      <c r="A24" s="1"/>
     </row>
     <row r="25" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="82.8" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>28</v>
-      </c>
+      <c r="A25" s="1"/>
+    </row>
+    <row r="26" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A26" s="1"/>
+    </row>
+    <row r="27" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A27" s="1"/>
     </row>
     <row r="28" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="55.2" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="138" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>4</v>
-      </c>
+      <c r="A28" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -988,8 +829,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D394C38-F921-48A4-941A-34759F663F0D}">
   <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1004,31 +845,31 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="G1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I1" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="I1" s="5" t="s">
-        <v>43</v>
-      </c>
       <c r="J1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="K1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -1037,21 +878,21 @@
         <v>0</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E2" s="5"/>
       <c r="F2">
         <v>0</v>
       </c>
       <c r="G2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="I2" s="5"/>
       <c r="J2">
         <v>0</v>
       </c>
       <c r="K2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -1060,21 +901,21 @@
         <v>1</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E3" s="5"/>
       <c r="F3">
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="I3" s="5"/>
       <c r="J3">
         <v>1</v>
       </c>
       <c r="K3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="41.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -1083,7 +924,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E4" s="5"/>
       <c r="I4" s="5"/>
@@ -1091,7 +932,7 @@
         <v>2</v>
       </c>
       <c r="K4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -1100,7 +941,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E5" s="5"/>
       <c r="I5" s="5"/>
@@ -1108,7 +949,7 @@
         <v>3</v>
       </c>
       <c r="K5" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -1117,7 +958,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E6" s="5"/>
       <c r="I6" s="5"/>
@@ -1125,7 +966,7 @@
         <v>4</v>
       </c>
       <c r="K6" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix the original books' bug and update API doc
</commit_message>
<xml_diff>
--- a/DOC/API.xlsx
+++ b/DOC/API.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Develop\nodejs\node_global\IFN711 Team72\DOC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1864A82B-3738-4E5B-B4D3-976C69090293}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C8A5EF3-B136-4BF1-9625-476B5112DB1C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="54">
   <si>
     <t>/api/user/login</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -36,10 +36,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>/api/user/insertUser</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>API</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -48,14 +44,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>/api/user/updateInfo</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/api/user/updateExp</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>/api/origin/list</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -100,163 +88,210 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve"> username 
- nickname 
- password 
- address 
- email 
- phone 
- firstname 
- lastname 
- experience </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> username  
- experience </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> id 
- trans_num 
- download_loc 
- status 
- status_info </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  id 
-  download_loc 
-  status 
-  status_info 
-  startdate 
-  enddate 
-  translation_reviewer_id 
-  cultrue_reviewer_id 
-  copy_reviewer_id 
-  admin_id </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> username
- role
- rolename
- nickname 
- password
- address 
- email 
- phone 
- firstname 
- lastname </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve"> username 
- password</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <t>users</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>role</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>rolename</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>translator</t>
+  </si>
+  <si>
+    <t>translation reivewer</t>
+  </si>
+  <si>
+    <t>culture reviewer</t>
+  </si>
+  <si>
+    <t>copy reviewer</t>
+  </si>
+  <si>
+    <t>original_books</t>
+  </si>
+  <si>
+    <t>status</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>status_info</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>locked</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>normal</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>translated_books</t>
+  </si>
+  <si>
+    <t>published</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>being translated</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>being translation viewed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>being culture reviewed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>being copy reviewed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/api/origin/add</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/api/user/insert</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/api/user/update</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/api/wait/list</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/api/wait/del</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/api/wait/add</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GET</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>POST</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">name
+original_id
+original_language
+target_language
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>name
+original_id
+original_language
+target_language
+image</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>username
+password</t>
+  </si>
+  <si>
+    <t>username
+role
+rolename
+password
+address
+email
+phone
+firstname
+lastname</t>
+  </si>
+  <si>
+    <t>username
+title
+password
+address
+email
+phone
+firstname
+lastname
+experience
+translation_num
+review_num
+can_review
+status</t>
+  </si>
+  <si>
+    <t>original_id
+language
+translator_id
+translation_reviewer_id
+cultrue_reviewer_id
+status</t>
   </si>
   <si>
     <t>name
 author
-publisher
-category
+language
 trans_num
 status</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>original_id
+    <t>name
+author
 language
- translator_id
- translation_reviewer_id
- cultrue_reviewer_id
- status</t>
+download_loc
+image</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id
+trans_num
+download_loc
+status
+status_info
+image</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>translator_id
-  original_id 
-  language
-  startdate</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>users</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>role</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>rolename</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>admin</t>
-  </si>
-  <si>
-    <t>translator</t>
-  </si>
-  <si>
-    <t>translation reivewer</t>
-  </si>
-  <si>
-    <t>culture reviewer</t>
-  </si>
-  <si>
-    <t>copy reviewer</t>
-  </si>
-  <si>
-    <t>original_books</t>
-  </si>
-  <si>
-    <t>status</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>status_info</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>locked</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>normal</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>translated_books</t>
-  </si>
-  <si>
-    <t>published</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>being translated</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>being translation viewed</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>being culture reviewed</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>being copy reviewed</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/api/origin/add</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve"> name
- publisher
- author
- category 
- language
- download_loc
- publish_time</t>
+original_id
+language
+startdate
+image
+name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id
+name
+download_loc
+status
+status_info
+startdate
+enddate
+translation_reviewer_id
+cultrue_reviewer_idadmin_id
+admin_id
+image</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -606,10 +641,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -622,10 +657,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>3</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
@@ -636,170 +671,184 @@
         <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="138" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="124.2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>35</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="124.2" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="179.4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="48" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:3" ht="69" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="C6" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="82.8" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="B7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="2" t="s">
+    </row>
+    <row r="8" spans="1:3" ht="82.8" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="B8" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>10</v>
+        <v>1</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="69" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="52.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+    </row>
+    <row r="12" spans="1:3" ht="82.8" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="96.6" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="B13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="82.8" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-    </row>
-    <row r="13" spans="1:3" ht="82.8" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="B14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="151.80000000000001" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="B15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="55.2" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="138" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="B16" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-    </row>
-    <row r="19" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
+      <c r="C16" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="48.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+    </row>
+    <row r="18" spans="1:3" ht="69" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="69" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="20" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
+      <c r="A20" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="21" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
     </row>
-    <row r="22" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
-    </row>
     <row r="23" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
     </row>
@@ -814,9 +863,6 @@
     </row>
     <row r="27" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
-    </row>
-    <row r="28" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A28" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -845,31 +891,31 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="B1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I1" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="F1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G1" t="s">
-        <v>37</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>40</v>
-      </c>
       <c r="J1" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="K1" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -878,21 +924,21 @@
         <v>0</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="E2" s="5"/>
       <c r="F2">
         <v>0</v>
       </c>
       <c r="G2" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="I2" s="5"/>
       <c r="J2">
         <v>0</v>
       </c>
       <c r="K2" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -901,21 +947,21 @@
         <v>1</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="E3" s="5"/>
       <c r="F3">
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="I3" s="5"/>
       <c r="J3">
         <v>1</v>
       </c>
       <c r="K3" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="41.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -924,7 +970,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="E4" s="5"/>
       <c r="I4" s="5"/>
@@ -932,7 +978,7 @@
         <v>2</v>
       </c>
       <c r="K4" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -941,7 +987,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="E5" s="5"/>
       <c r="I5" s="5"/>
@@ -949,7 +995,7 @@
         <v>3</v>
       </c>
       <c r="K5" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -958,7 +1004,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="E6" s="5"/>
       <c r="I6" s="5"/>
@@ -966,7 +1012,7 @@
         <v>4</v>
       </c>
       <c r="K6" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>